<commit_message>
Exception Handling notes and examples
</commit_message>
<xml_diff>
--- a/Updates.xlsx
+++ b/Updates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java Full Stack\JAVA\CORE\KTG\Ranjith\2023 march batch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6AAD09B-C684-466E-A9A1-678F67D70BFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C97577-5273-420B-BA83-414CE18F80CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="77">
   <si>
     <t>Concepts</t>
   </si>
@@ -178,9 +178,6 @@
     <t>2:05pm-5:00pm</t>
   </si>
   <si>
-    <t>multi threading</t>
-  </si>
-  <si>
     <t>collections</t>
   </si>
   <si>
@@ -251,6 +248,15 @@
   </si>
   <si>
     <t>10:30-11:25 PM</t>
+  </si>
+  <si>
+    <t>day-23</t>
+  </si>
+  <si>
+    <t>Exception handling</t>
+  </si>
+  <si>
+    <t>10:40-11:25 PM</t>
   </si>
 </sst>
 </file>
@@ -693,7 +699,7 @@
   <dimension ref="A3:I167"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="F28" sqref="F28:F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -835,7 +841,7 @@
     </row>
     <row r="11" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D11" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E11" s="6">
         <v>45016</v>
@@ -851,7 +857,7 @@
     </row>
     <row r="12" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D12" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E12" s="6">
         <v>45019</v>
@@ -867,7 +873,7 @@
     </row>
     <row r="13" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D13" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E13" s="6">
         <v>45022</v>
@@ -883,7 +889,7 @@
     </row>
     <row r="14" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D14" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E14" s="6">
         <v>45023</v>
@@ -899,7 +905,7 @@
     </row>
     <row r="15" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D15" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E15" s="8">
         <v>45026</v>
@@ -915,7 +921,7 @@
     </row>
     <row r="16" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D16" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E16" s="8">
         <v>45027</v>
@@ -933,7 +939,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D17" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E17" s="8">
         <v>45028</v>
@@ -947,7 +953,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D18" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E18" s="8">
         <v>45035</v>
@@ -961,7 +967,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D19" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E19" s="8">
         <v>45040</v>
@@ -978,7 +984,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="9"/>
       <c r="D20" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E20" s="8">
         <v>45042</v>
@@ -996,7 +1002,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D21" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E21" s="8">
         <v>45044</v>
@@ -1012,7 +1018,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D22" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E22" s="8">
         <v>45048</v>
@@ -1028,7 +1034,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D23" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E23" s="8">
         <v>45051</v>
@@ -1044,7 +1050,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D24" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E24" s="8">
         <v>45052</v>
@@ -1060,43 +1066,49 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D25" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E25" s="8">
         <v>45059</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D26" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E26" s="8">
         <v>45061</v>
       </c>
       <c r="F26" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="G26" s="5" t="s">
         <v>73</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>74</v>
       </c>
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D27" s="4"/>
-      <c r="E27" s="5"/>
+      <c r="D27" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E27" s="8">
+        <v>45065</v>
+      </c>
       <c r="F27" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="G27" s="5"/>
+        <v>75</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>76</v>
+      </c>
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
     </row>
@@ -1104,7 +1116,7 @@
       <c r="D28" s="4"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
@@ -1114,7 +1126,7 @@
       <c r="D29" s="4"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
@@ -1124,7 +1136,7 @@
       <c r="D30" s="4"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
@@ -1134,7 +1146,7 @@
       <c r="D31" s="4"/>
       <c r="E31" s="8"/>
       <c r="F31" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
@@ -1144,7 +1156,7 @@
       <c r="D32" s="4"/>
       <c r="E32" s="8"/>
       <c r="F32" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>

</xml_diff>

<commit_message>
Day-30 SPring boot Examples
</commit_message>
<xml_diff>
--- a/Updates.xlsx
+++ b/Updates.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java Full Stack\JAVA\CORE\KTG\Ranjith\2023 march batch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C97577-5273-420B-BA83-414CE18F80CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23C32A76-7D87-4781-A3EF-1213C7A373BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="92">
   <si>
     <t>Concepts</t>
   </si>
@@ -178,18 +178,6 @@
     <t>2:05pm-5:00pm</t>
   </si>
   <si>
-    <t>collections</t>
-  </si>
-  <si>
-    <t xml:space="preserve">java8 </t>
-  </si>
-  <si>
-    <t>case study</t>
-  </si>
-  <si>
-    <t>database ,jpa,hibernate,spring ,springboot</t>
-  </si>
-  <si>
     <t>day-7</t>
   </si>
   <si>
@@ -257,6 +245,63 @@
   </si>
   <si>
     <t>10:40-11:25 PM</t>
+  </si>
+  <si>
+    <t>day-24</t>
+  </si>
+  <si>
+    <t>12:45PM-1:52PM</t>
+  </si>
+  <si>
+    <t>day-25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">multi threading </t>
+  </si>
+  <si>
+    <t>Inter Thread Communication,collections(List,Set)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Map(Case study)</t>
+  </si>
+  <si>
+    <t>Java8 features</t>
+  </si>
+  <si>
+    <t>day-26</t>
+  </si>
+  <si>
+    <t>day-27</t>
+  </si>
+  <si>
+    <t>12:30PM -1:45PM</t>
+  </si>
+  <si>
+    <t>12:45PM-1:50PM</t>
+  </si>
+  <si>
+    <t>1:00pm-2:15pm</t>
+  </si>
+  <si>
+    <t>day-28</t>
+  </si>
+  <si>
+    <t>day-29</t>
+  </si>
+  <si>
+    <t>day-30</t>
+  </si>
+  <si>
+    <t>jpa,hibernate</t>
+  </si>
+  <si>
+    <t>11:15-2:00Pm</t>
+  </si>
+  <si>
+    <t>spring core,spring jpa,springmvc,spring boot case study</t>
+  </si>
+  <si>
+    <t>1:05pm-3:45Pm</t>
   </si>
 </sst>
 </file>
@@ -696,10 +741,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:I167"/>
+  <dimension ref="A3:I168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28:F30"/>
+    <sheetView tabSelected="1" topLeftCell="C14" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -841,7 +886,7 @@
     </row>
     <row r="11" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D11" s="4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E11" s="6">
         <v>45016</v>
@@ -857,7 +902,7 @@
     </row>
     <row r="12" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D12" s="4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E12" s="6">
         <v>45019</v>
@@ -873,7 +918,7 @@
     </row>
     <row r="13" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D13" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E13" s="6">
         <v>45022</v>
@@ -889,7 +934,7 @@
     </row>
     <row r="14" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D14" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E14" s="6">
         <v>45023</v>
@@ -905,7 +950,7 @@
     </row>
     <row r="15" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D15" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E15" s="8">
         <v>45026</v>
@@ -921,7 +966,7 @@
     </row>
     <row r="16" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D16" s="4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E16" s="8">
         <v>45027</v>
@@ -939,7 +984,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D17" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E17" s="8">
         <v>45028</v>
@@ -953,7 +998,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D18" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E18" s="8">
         <v>45035</v>
@@ -967,7 +1012,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D19" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E19" s="8">
         <v>45040</v>
@@ -984,7 +1029,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="9"/>
       <c r="D20" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E20" s="8">
         <v>45042</v>
@@ -1002,7 +1047,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D21" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E21" s="8">
         <v>45044</v>
@@ -1018,7 +1063,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D22" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E22" s="8">
         <v>45048</v>
@@ -1034,7 +1079,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D23" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E23" s="8">
         <v>45051</v>
@@ -1050,7 +1095,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D24" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E24" s="8">
         <v>45052</v>
@@ -1066,115 +1111,161 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D25" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E25" s="8">
         <v>45059</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D26" s="4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E26" s="8">
         <v>45061</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D27" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E27" s="8">
         <v>45065</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D28" s="4"/>
-      <c r="E28" s="5"/>
+      <c r="D28" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E28" s="8">
+        <v>45069</v>
+      </c>
       <c r="F28" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="G28" s="5"/>
+        <v>76</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>74</v>
+      </c>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D29" s="4"/>
-      <c r="E29" s="5"/>
+      <c r="D29" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E29" s="8">
+        <v>45070</v>
+      </c>
       <c r="F29" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G29" s="5"/>
+        <v>77</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D30" s="4"/>
-      <c r="E30" s="5"/>
+      <c r="D30" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E30" s="8">
+        <v>45071</v>
+      </c>
       <c r="F30" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="G30" s="5"/>
+        <v>78</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D31" s="4"/>
-      <c r="E31" s="8"/>
+      <c r="D31" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E31" s="8">
+        <v>45072</v>
+      </c>
       <c r="F31" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="G31" s="5"/>
+        <v>79</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>84</v>
+      </c>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D32" s="4"/>
-      <c r="E32" s="8"/>
+      <c r="D32" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E32" s="8">
+        <v>45077</v>
+      </c>
       <c r="F32" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="G32" s="5"/>
+        <v>79</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>84</v>
+      </c>
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
     </row>
     <row r="33" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D33" s="4"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
+      <c r="D33" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E33" s="8">
+        <v>45079</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>89</v>
+      </c>
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
     </row>
     <row r="34" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D34" s="4"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
+      <c r="D34" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E34" s="8">
+        <v>45087</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>91</v>
+      </c>
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
     </row>
@@ -1292,7 +1383,7 @@
     </row>
     <row r="49" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D49" s="4"/>
-      <c r="E49" s="5"/>
+      <c r="E49" s="8"/>
       <c r="F49" s="5"/>
       <c r="G49" s="5"/>
       <c r="H49" s="5"/>
@@ -2235,11 +2326,19 @@
       <c r="I166" s="5"/>
     </row>
     <row r="167" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D167" s="4"/>
       <c r="E167" s="5"/>
       <c r="F167" s="5"/>
       <c r="G167" s="5"/>
       <c r="H167" s="5"/>
       <c r="I167" s="5"/>
+    </row>
+    <row r="168" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="E168" s="5"/>
+      <c r="F168" s="5"/>
+      <c r="G168" s="5"/>
+      <c r="H168" s="5"/>
+      <c r="I168" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>